<commit_message>
Flesh out the tutorial a bit.
</commit_message>
<xml_diff>
--- a/external-docs/docs/arch-diagram.xlsx
+++ b/external-docs/docs/arch-diagram.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mike/Corda/conclave2/external-docs/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{331CB8EB-52B5-774D-B364-4733984E8B3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CDF2F46-1FEA-2446-B403-A8E157E3CEDF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{2ED672D7-C865-D444-BDEA-C0A5C51D3721}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$3:$J$9</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -355,13 +358,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>1</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>86985</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>817672</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>144976</xdr:rowOff>
@@ -414,13 +417,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>11598</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>173973</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>806073</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>173973</xdr:rowOff>
@@ -473,13 +476,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>417534</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>11598</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>417534</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>173973</xdr:rowOff>
@@ -830,84 +833,85 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61BDCF0D-AF12-514B-A4F7-D1238802FD19}">
-  <dimension ref="A3:H9"/>
+  <dimension ref="B3:I9"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="218" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="E3" s="4" t="s">
+      <c r="C3" s="10"/>
+      <c r="F3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="11"/>
-      <c r="B4" s="12"/>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B4" s="11"/>
+      <c r="C4" s="12"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="11"/>
-      <c r="B5" s="12"/>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B5" s="11"/>
+      <c r="C5" s="12"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="11"/>
-      <c r="B6" s="12"/>
-      <c r="D6" s="7" t="s">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B6" s="11"/>
+      <c r="C6" s="12"/>
+      <c r="E6" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="1" t="s">
+      <c r="F6" s="7"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="13"/>
-      <c r="B7" s="14"/>
-      <c r="D7" s="7"/>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B7" s="13"/>
+      <c r="C7" s="14"/>
       <c r="E7" s="7"/>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="7"/>
+      <c r="G7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G7" s="1"/>
       <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D8" s="8" t="s">
+    <row r="8" spans="2:9" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E8" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="E8" s="8"/>
       <c r="F8" s="8"/>
-      <c r="G8" s="1"/>
+      <c r="G8" s="8"/>
       <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
     </row>
-    <row r="9" spans="1:8" ht="37" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D9" s="3" t="s">
+    <row r="9" spans="2:9" ht="37" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E9" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="A3:B7"/>
-    <mergeCell ref="D9:H9"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="D6:E7"/>
-    <mergeCell ref="G6:H8"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="B3:C7"/>
+    <mergeCell ref="E9:I9"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="E6:F7"/>
+    <mergeCell ref="H6:I8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>